<commit_message>
Pricesheet for Thu 18 Feb 2021 23:15:17 CAT
</commit_message>
<xml_diff>
--- a/xls-daily-price-sheets/18-02-2021.xlsx
+++ b/xls-daily-price-sheets/18-02-2021.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="157">
   <si>
     <t>Company Name</t>
   </si>
@@ -55,9 +55,6 @@
     <t>Dairibord Holdings Limited</t>
   </si>
   <si>
-    <t>Dawn Properties Limited</t>
-  </si>
-  <si>
     <t>Delta Corporation Limited</t>
   </si>
   <si>
@@ -178,370 +175,316 @@
     <t>Opening Price</t>
   </si>
   <si>
-    <t>30.5429</t>
-  </si>
-  <si>
-    <t>1.5411</t>
-  </si>
-  <si>
-    <t>6.8176</t>
+    <t>34.8000</t>
+  </si>
+  <si>
+    <t>1.5315</t>
+  </si>
+  <si>
+    <t>6.9375</t>
+  </si>
+  <si>
+    <t>2.3383</t>
+  </si>
+  <si>
+    <t>17.0000</t>
+  </si>
+  <si>
+    <t>4.8155</t>
+  </si>
+  <si>
+    <t>874.0000</t>
+  </si>
+  <si>
+    <t>95.0000</t>
+  </si>
+  <si>
+    <t>11.0173</t>
+  </si>
+  <si>
+    <t>90.5000</t>
+  </si>
+  <si>
+    <t>19.1167</t>
+  </si>
+  <si>
+    <t>41.9251</t>
+  </si>
+  <si>
+    <t>18.3246</t>
+  </si>
+  <si>
+    <t>3.2583</t>
+  </si>
+  <si>
+    <t>25.0500</t>
+  </si>
+  <si>
+    <t>2.9188</t>
+  </si>
+  <si>
+    <t>1.8686</t>
+  </si>
+  <si>
+    <t>15.0000</t>
+  </si>
+  <si>
+    <t>6.0000</t>
+  </si>
+  <si>
+    <t>0.2053</t>
+  </si>
+  <si>
+    <t>0.3105</t>
+  </si>
+  <si>
+    <t>95.0538</t>
+  </si>
+  <si>
+    <t>56.0022</t>
+  </si>
+  <si>
+    <t>23.0000</t>
+  </si>
+  <si>
+    <t>0.9650</t>
+  </si>
+  <si>
+    <t>15.2813</t>
+  </si>
+  <si>
+    <t>0.0745</t>
+  </si>
+  <si>
+    <t>40.0035</t>
+  </si>
+  <si>
+    <t>6.0100</t>
+  </si>
+  <si>
+    <t>184.8000</t>
+  </si>
+  <si>
+    <t>0.5675</t>
+  </si>
+  <si>
+    <t>16.0009</t>
+  </si>
+  <si>
+    <t>29.3042</t>
+  </si>
+  <si>
+    <t>24.0000</t>
+  </si>
+  <si>
+    <t>1.5975</t>
+  </si>
+  <si>
+    <t>19.7660</t>
+  </si>
+  <si>
+    <t>24.1061</t>
+  </si>
+  <si>
+    <t>18.5247</t>
+  </si>
+  <si>
+    <t>0.4721</t>
+  </si>
+  <si>
+    <t>0.7500</t>
+  </si>
+  <si>
+    <t>44.9480</t>
+  </si>
+  <si>
+    <t>1.3000</t>
+  </si>
+  <si>
+    <t>3.1975</t>
+  </si>
+  <si>
+    <t>0.5519</t>
+  </si>
+  <si>
+    <t>40.0000</t>
+  </si>
+  <si>
+    <t>0.0002</t>
+  </si>
+  <si>
+    <t>1.1200</t>
+  </si>
+  <si>
+    <t>8.3000</t>
+  </si>
+  <si>
+    <t>2.1500</t>
+  </si>
+  <si>
+    <t>Closing Price</t>
+  </si>
+  <si>
+    <t>1.7314</t>
+  </si>
+  <si>
+    <t>6.9500</t>
   </si>
   <si>
     <t>2.3500</t>
   </si>
   <si>
-    <t>17.0000</t>
-  </si>
-  <si>
-    <t>4.8025</t>
-  </si>
-  <si>
-    <t>874.0000</t>
-  </si>
-  <si>
-    <t>95.0000</t>
-  </si>
-  <si>
-    <t>11.1010</t>
-  </si>
-  <si>
-    <t>99.7500</t>
-  </si>
-  <si>
-    <t>19.3855</t>
-  </si>
-  <si>
-    <t>0.4000</t>
-  </si>
-  <si>
-    <t>42.4071</t>
-  </si>
-  <si>
-    <t>18.8093</t>
-  </si>
-  <si>
-    <t>3.2591</t>
-  </si>
-  <si>
-    <t>25.0816</t>
-  </si>
-  <si>
-    <t>2.8636</t>
-  </si>
-  <si>
-    <t>1.9320</t>
-  </si>
-  <si>
-    <t>15.0330</t>
-  </si>
-  <si>
-    <t>5.7500</t>
-  </si>
-  <si>
-    <t>0.2053</t>
-  </si>
-  <si>
-    <t>0.3105</t>
-  </si>
-  <si>
-    <t>55.9781</t>
-  </si>
-  <si>
-    <t>23.0000</t>
-  </si>
-  <si>
-    <t>1.0214</t>
+    <t>5.5000</t>
+  </si>
+  <si>
+    <t>10.9260</t>
+  </si>
+  <si>
+    <t>19.0000</t>
+  </si>
+  <si>
+    <t>42.0000</t>
+  </si>
+  <si>
+    <t>17.4966</t>
+  </si>
+  <si>
+    <t>3.2500</t>
+  </si>
+  <si>
+    <t>26.5000</t>
+  </si>
+  <si>
+    <t>2.5673</t>
+  </si>
+  <si>
+    <t>1.9039</t>
+  </si>
+  <si>
+    <t>0.2100</t>
+  </si>
+  <si>
+    <t>1.1575</t>
   </si>
   <si>
     <t>16.0000</t>
   </si>
   <si>
-    <t>0.0749</t>
-  </si>
-  <si>
-    <t>42.0000</t>
-  </si>
-  <si>
-    <t>6.1008</t>
-  </si>
-  <si>
-    <t>184.8000</t>
-  </si>
-  <si>
-    <t>0.3945</t>
-  </si>
-  <si>
-    <t>6.0000</t>
-  </si>
-  <si>
-    <t>17.3360</t>
-  </si>
-  <si>
-    <t>29.9992</t>
-  </si>
-  <si>
-    <t>20.0000</t>
-  </si>
-  <si>
-    <t>1.7000</t>
-  </si>
-  <si>
-    <t>22.2426</t>
-  </si>
-  <si>
-    <t>25.0000</t>
-  </si>
-  <si>
-    <t>20.9989</t>
-  </si>
-  <si>
-    <t>0.5056</t>
-  </si>
-  <si>
-    <t>0.7525</t>
-  </si>
-  <si>
-    <t>44.9480</t>
-  </si>
-  <si>
-    <t>1.3000</t>
-  </si>
-  <si>
-    <t>2.6650</t>
-  </si>
-  <si>
-    <t>0.5500</t>
-  </si>
-  <si>
-    <t>40.0000</t>
-  </si>
-  <si>
-    <t>0.0002</t>
-  </si>
-  <si>
-    <t>1.1200</t>
-  </si>
-  <si>
-    <t>8.3000</t>
-  </si>
-  <si>
-    <t>2.3900</t>
-  </si>
-  <si>
-    <t>Closing Price</t>
-  </si>
-  <si>
-    <t>34.8000</t>
-  </si>
-  <si>
-    <t>1.5315</t>
-  </si>
-  <si>
-    <t>6.9375</t>
-  </si>
-  <si>
-    <t>2.3383</t>
-  </si>
-  <si>
-    <t>4.8155</t>
-  </si>
-  <si>
-    <t>11.0173</t>
-  </si>
-  <si>
-    <t>90.5000</t>
-  </si>
-  <si>
-    <t>19.1167</t>
-  </si>
-  <si>
-    <t>41.9251</t>
-  </si>
-  <si>
-    <t>18.3246</t>
-  </si>
-  <si>
-    <t>3.2583</t>
-  </si>
-  <si>
-    <t>25.0500</t>
-  </si>
-  <si>
-    <t>2.9188</t>
-  </si>
-  <si>
-    <t>1.8686</t>
-  </si>
-  <si>
-    <t>15.0000</t>
-  </si>
-  <si>
-    <t>95.0538</t>
-  </si>
-  <si>
-    <t>56.0022</t>
-  </si>
-  <si>
-    <t>0.9650</t>
-  </si>
-  <si>
-    <t>15.2813</t>
-  </si>
-  <si>
-    <t>0.0745</t>
-  </si>
-  <si>
-    <t>40.0035</t>
-  </si>
-  <si>
-    <t>6.0100</t>
-  </si>
-  <si>
-    <t>0.4730</t>
-  </si>
-  <si>
-    <t>16.0009</t>
-  </si>
-  <si>
-    <t>29.3042</t>
-  </si>
-  <si>
-    <t>24.0000</t>
-  </si>
-  <si>
-    <t>1.5975</t>
-  </si>
-  <si>
-    <t>19.7660</t>
-  </si>
-  <si>
-    <t>24.1061</t>
-  </si>
-  <si>
-    <t>18.5247</t>
-  </si>
-  <si>
-    <t>0.4721</t>
-  </si>
-  <si>
-    <t>0.7500</t>
-  </si>
-  <si>
-    <t>3.1975</t>
-  </si>
-  <si>
-    <t>0.5519</t>
-  </si>
-  <si>
-    <t>2.1500</t>
+    <t>0.0720</t>
+  </si>
+  <si>
+    <t>41.7500</t>
+  </si>
+  <si>
+    <t>7.2000</t>
+  </si>
+  <si>
+    <t>16.4122</t>
+  </si>
+  <si>
+    <t>30.0000</t>
+  </si>
+  <si>
+    <t>1.6645</t>
+  </si>
+  <si>
+    <t>21.0000</t>
+  </si>
+  <si>
+    <t>19.7857</t>
+  </si>
+  <si>
+    <t>0.5060</t>
+  </si>
+  <si>
+    <t>44.9500</t>
+  </si>
+  <si>
+    <t>1.5000</t>
+  </si>
+  <si>
+    <t>0.5668</t>
+  </si>
+  <si>
+    <t>8.2000</t>
   </si>
   <si>
     <t>Total Traded Volume</t>
   </si>
   <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>5100</t>
+  </si>
+  <si>
+    <t>1200</t>
+  </si>
+  <si>
+    <t>4600</t>
+  </si>
+  <si>
+    <t>38500</t>
+  </si>
+  <si>
+    <t>800</t>
+  </si>
+  <si>
+    <t>2500</t>
+  </si>
+  <si>
+    <t>400</t>
+  </si>
+  <si>
+    <t>13900</t>
+  </si>
+  <si>
+    <t>108600</t>
+  </si>
+  <si>
     <t>100</t>
   </si>
   <si>
-    <t>59200</t>
-  </si>
-  <si>
-    <t>8800</t>
-  </si>
-  <si>
-    <t>4700</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>22900</t>
-  </si>
-  <si>
-    <t>1035700</t>
-  </si>
-  <si>
-    <t>400</t>
-  </si>
-  <si>
-    <t>300</t>
-  </si>
-  <si>
-    <t>1146000</t>
-  </si>
-  <si>
-    <t>463900</t>
-  </si>
-  <si>
-    <t>3000</t>
-  </si>
-  <si>
-    <t>3200</t>
-  </si>
-  <si>
-    <t>1600</t>
-  </si>
-  <si>
-    <t>21200</t>
+    <t>1500</t>
+  </si>
+  <si>
+    <t>689700</t>
   </si>
   <si>
     <t>500</t>
   </si>
   <si>
-    <t>800</t>
-  </si>
-  <si>
-    <t>18600</t>
-  </si>
-  <si>
-    <t>329900</t>
-  </si>
-  <si>
-    <t>104900</t>
-  </si>
-  <si>
-    <t>6010000</t>
-  </si>
-  <si>
-    <t>57700</t>
-  </si>
-  <si>
-    <t>3100</t>
-  </si>
-  <si>
-    <t>2100</t>
-  </si>
-  <si>
-    <t>635200</t>
-  </si>
-  <si>
-    <t>23900</t>
-  </si>
-  <si>
-    <t>8500</t>
-  </si>
-  <si>
-    <t>7200</t>
-  </si>
-  <si>
-    <t>6600</t>
-  </si>
-  <si>
-    <t>589400</t>
-  </si>
-  <si>
-    <t>105800</t>
-  </si>
-  <si>
-    <t>1300</t>
-  </si>
-  <si>
-    <t>48000</t>
-  </si>
-  <si>
-    <t>756500</t>
-  </si>
-  <si>
-    <t>23100</t>
+    <t>17400</t>
+  </si>
+  <si>
+    <t>2116900</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>1100</t>
+  </si>
+  <si>
+    <t>4900</t>
+  </si>
+  <si>
+    <t>1400</t>
+  </si>
+  <si>
+    <t>11800</t>
+  </si>
+  <si>
+    <t>68400</t>
+  </si>
+  <si>
+    <t>2800</t>
+  </si>
+  <si>
+    <t>24800</t>
+  </si>
+  <si>
+    <t>7900</t>
   </si>
 </sst>
 </file>
@@ -899,7 +842,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -924,13 +867,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D2" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -943,13 +886,13 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" t="s">
-        <v>105</v>
+        <v>53</v>
       </c>
       <c r="D6" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -957,13 +900,13 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D7" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -971,13 +914,13 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C8" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D8" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -985,13 +928,13 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C9" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D9" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -999,13 +942,13 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D10" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1013,13 +956,13 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C11" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D11" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1027,13 +970,13 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D12" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1041,13 +984,13 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D13" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1055,13 +998,13 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C14" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D14" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1069,13 +1012,13 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C15" t="s">
-        <v>111</v>
+        <v>62</v>
       </c>
       <c r="D15" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1083,13 +1026,13 @@
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C16" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D16" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1097,13 +1040,13 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C17" t="s">
-        <v>65</v>
+        <v>109</v>
       </c>
       <c r="D17" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1111,13 +1054,13 @@
         <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C18" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D18" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1125,13 +1068,13 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C19" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D19" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1139,13 +1082,13 @@
         <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C20" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D20" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1153,13 +1096,13 @@
         <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C21" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D21" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1167,13 +1110,13 @@
         <v>18</v>
       </c>
       <c r="B22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C22" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D22" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1181,13 +1124,13 @@
         <v>19</v>
       </c>
       <c r="B23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C23" t="s">
-        <v>118</v>
+        <v>70</v>
       </c>
       <c r="D23" t="s">
-        <v>155</v>
+        <v>132</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1195,13 +1138,13 @@
         <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C24" t="s">
-        <v>119</v>
+        <v>71</v>
       </c>
       <c r="D24" t="s">
-        <v>156</v>
+        <v>132</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1209,13 +1152,13 @@
         <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C25" t="s">
-        <v>85</v>
+        <v>115</v>
       </c>
       <c r="D25" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1223,13 +1166,13 @@
         <v>22</v>
       </c>
       <c r="B26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D26" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1237,13 +1180,13 @@
         <v>23</v>
       </c>
       <c r="B27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D27" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1251,13 +1194,13 @@
         <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="C28" t="s">
-        <v>120</v>
+        <v>75</v>
       </c>
       <c r="D28" t="s">
-        <v>158</v>
+        <v>132</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1268,10 +1211,10 @@
         <v>76</v>
       </c>
       <c r="C29" t="s">
-        <v>121</v>
+        <v>76</v>
       </c>
       <c r="D29" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1282,10 +1225,10 @@
         <v>77</v>
       </c>
       <c r="C30" t="s">
-        <v>77</v>
+        <v>116</v>
       </c>
       <c r="D30" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1296,10 +1239,10 @@
         <v>78</v>
       </c>
       <c r="C31" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D31" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1310,10 +1253,10 @@
         <v>79</v>
       </c>
       <c r="C32" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D32" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1324,10 +1267,10 @@
         <v>80</v>
       </c>
       <c r="C33" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D33" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1338,10 +1281,10 @@
         <v>81</v>
       </c>
       <c r="C34" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D34" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1352,10 +1295,10 @@
         <v>82</v>
       </c>
       <c r="C35" t="s">
-        <v>126</v>
+        <v>82</v>
       </c>
       <c r="D35" t="s">
-        <v>163</v>
+        <v>132</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1369,7 +1312,7 @@
         <v>83</v>
       </c>
       <c r="D36" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1377,13 +1320,13 @@
         <v>33</v>
       </c>
       <c r="B37" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="C37" t="s">
-        <v>127</v>
+        <v>71</v>
       </c>
       <c r="D37" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1391,13 +1334,13 @@
         <v>34</v>
       </c>
       <c r="B38" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C38" t="s">
-        <v>85</v>
+        <v>121</v>
       </c>
       <c r="D38" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1405,13 +1348,13 @@
         <v>35</v>
       </c>
       <c r="B39" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C39" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D39" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1419,13 +1362,13 @@
         <v>36</v>
       </c>
       <c r="B40" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C40" t="s">
-        <v>129</v>
+        <v>86</v>
       </c>
       <c r="D40" t="s">
-        <v>166</v>
+        <v>132</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1433,13 +1376,13 @@
         <v>37</v>
       </c>
       <c r="B41" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C41" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="D41" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1447,13 +1390,13 @@
         <v>38</v>
       </c>
       <c r="B42" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C42" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D42" t="s">
-        <v>167</v>
+        <v>142</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1461,13 +1404,13 @@
         <v>39</v>
       </c>
       <c r="B43" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C43" t="s">
-        <v>132</v>
+        <v>89</v>
       </c>
       <c r="D43" t="s">
-        <v>168</v>
+        <v>132</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1475,13 +1418,13 @@
         <v>40</v>
       </c>
       <c r="B44" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C44" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="D44" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1489,13 +1432,13 @@
         <v>41</v>
       </c>
       <c r="B45" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C45" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="D45" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1503,13 +1446,13 @@
         <v>42</v>
       </c>
       <c r="B46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C46" t="s">
-        <v>135</v>
+        <v>92</v>
       </c>
       <c r="D46" t="s">
-        <v>171</v>
+        <v>154</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1517,13 +1460,13 @@
         <v>43</v>
       </c>
       <c r="B47" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C47" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="D47" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1531,13 +1474,13 @@
         <v>44</v>
       </c>
       <c r="B48" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C48" t="s">
-        <v>95</v>
+        <v>128</v>
       </c>
       <c r="D48" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1545,13 +1488,13 @@
         <v>45</v>
       </c>
       <c r="B49" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C49" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D49" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1559,13 +1502,13 @@
         <v>46</v>
       </c>
       <c r="B50" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C50" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="D50" t="s">
-        <v>141</v>
+        <v>155</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1573,13 +1516,13 @@
         <v>47</v>
       </c>
       <c r="B51" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C51" t="s">
-        <v>138</v>
+        <v>97</v>
       </c>
       <c r="D51" t="s">
-        <v>173</v>
+        <v>142</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -1587,13 +1530,13 @@
         <v>48</v>
       </c>
       <c r="B52" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C52" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D52" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1601,13 +1544,13 @@
         <v>49</v>
       </c>
       <c r="B53" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C53" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D53" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -1615,13 +1558,13 @@
         <v>50</v>
       </c>
       <c r="B54" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C54" t="s">
-        <v>101</v>
+        <v>130</v>
       </c>
       <c r="D54" t="s">
-        <v>174</v>
+        <v>148</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1629,27 +1572,13 @@
         <v>51</v>
       </c>
       <c r="B55" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C55" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D55" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" t="s">
-        <v>52</v>
-      </c>
-      <c r="B56" t="s">
-        <v>103</v>
-      </c>
-      <c r="C56" t="s">
-        <v>139</v>
-      </c>
-      <c r="D56" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>